<commit_message>
update git ignore and summary sensitivity analysis
</commit_message>
<xml_diff>
--- a/Output/summary_detection_overlap_sensitivity.xlsx
+++ b/Output/summary_detection_overlap_sensitivity.xlsx
@@ -549,7 +549,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="n">
-        <v>0.769039</v>
+        <v>0.790387</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -689,11 +689,11 @@
         <v>22</v>
       </c>
       <c r="E4" t="n">
-        <v>0.802644</v>
+        <v>0.8136679999999999</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId</t>
+          <t>Multi_index_temp</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -759,7 +759,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="n">
-        <v>0.79619</v>
+        <v>0.808503</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7480290000000001</v>
+        <v>0.750807</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1249,7 +1249,7 @@
         <v>18</v>
       </c>
       <c r="E12" t="n">
-        <v>0.768211</v>
+        <v>0.779881</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="n">
-        <v>0.76441</v>
+        <v>0.772267</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1389,7 +1389,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="n">
-        <v>0.787216</v>
+        <v>0.796318</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1529,11 +1529,11 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>0.781295</v>
+        <v>0.804495</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId</t>
+          <t>Multi_index_HWMId_NL</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1809,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="E20" t="n">
-        <v>0.789013</v>
+        <v>0.80118</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>14</v>
       </c>
       <c r="E22" t="n">
-        <v>0.807359</v>
+        <v>0.808187</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2019,7 +2019,7 @@
         <v>13</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7888579999999999</v>
+        <v>0.799081</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>19</v>
       </c>
       <c r="E25" t="n">
-        <v>0.845897</v>
+        <v>0.8563460000000001</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2439,7 +2439,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>0.729481</v>
+        <v>0.732604</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2509,7 +2509,7 @@
         <v>8</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7384810000000001</v>
+        <v>0.751339</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>0.754733</v>
+        <v>0.76119</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2649,7 +2649,7 @@
         <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7566619999999999</v>
+        <v>0.7829970000000001</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2719,11 +2719,11 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7455540000000001</v>
+        <v>0.760463</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId</t>
+          <t>Pseudo_HWMId</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2789,7 +2789,7 @@
         <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>0.814148</v>
+        <v>0.8181389999999999</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -3209,11 +3209,11 @@
         <v>40</v>
       </c>
       <c r="E40" t="n">
-        <v>0.83302</v>
+        <v>0.842146</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId_pop_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3699,7 +3699,7 @@
         <v>14</v>
       </c>
       <c r="E47" t="n">
-        <v>0.759225</v>
+        <v>0.76602</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3839,11 +3839,11 @@
         <v>13</v>
       </c>
       <c r="E49" t="n">
-        <v>0.796385</v>
+        <v>0.8031</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId</t>
+          <t>Multi_index_temp</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -3909,7 +3909,7 @@
         <v>13</v>
       </c>
       <c r="E50" t="n">
-        <v>0.806552</v>
+        <v>0.812101</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -4049,7 +4049,7 @@
         <v>21</v>
       </c>
       <c r="E52" t="n">
-        <v>0.805584</v>
+        <v>0.819873</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -7455,17 +7455,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C110" t="n">
-        <v>738</v>
+        <v>504</v>
       </c>
       <c r="D110" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>0.811499</v>
+        <v>0.658578</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -7525,13 +7525,19 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C111" t="n">
-        <v>8</v>
+        <v>504</v>
       </c>
       <c r="D111" t="n">
-        <v>88</v>
-      </c>
-      <c r="E111" t="inlineStr"/>
-      <c r="F111" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.65907</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Multi_index_HWMId</t>
+        </is>
+      </c>
       <c r="G111" t="inlineStr">
         <is>
           <t>ERA5</t>
@@ -7589,17 +7595,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C112" t="n">
-        <v>537</v>
+        <v>504</v>
       </c>
       <c r="D112" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>0.682392</v>
+        <v>0.648145</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -7659,17 +7665,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C113" t="n">
-        <v>536</v>
+        <v>504</v>
       </c>
       <c r="D113" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>0.686997</v>
+        <v>0.658578</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -7729,17 +7735,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C114" t="n">
-        <v>579</v>
+        <v>504</v>
       </c>
       <c r="D114" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>0.798388</v>
+        <v>0.65907</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId_pop_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -7799,13 +7805,13 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C115" t="n">
-        <v>730</v>
+        <v>504</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>0.653942</v>
+        <v>0.648145</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -7869,17 +7875,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C116" t="n">
-        <v>728</v>
+        <v>504</v>
       </c>
       <c r="D116" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>0.831315</v>
+        <v>0.658578</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId_pop_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -7939,13 +7945,19 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C117" t="n">
-        <v>9</v>
+        <v>504</v>
       </c>
       <c r="D117" t="n">
-        <v>88</v>
-      </c>
-      <c r="E117" t="inlineStr"/>
-      <c r="F117" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.65907</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Multi_index_HWMId</t>
+        </is>
+      </c>
       <c r="G117" t="inlineStr">
         <is>
           <t>ERA5</t>
@@ -8006,14 +8018,14 @@
         <v>504</v>
       </c>
       <c r="D118" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>0.668525</v>
+        <v>0.648145</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -8073,17 +8085,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C119" t="n">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D119" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>0.6816489999999999</v>
+        <v>0.658578</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -8143,17 +8155,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C120" t="n">
-        <v>568</v>
+        <v>504</v>
       </c>
       <c r="D120" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>0.8220499999999999</v>
+        <v>0.65907</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId_pop_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -8213,13 +8225,13 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C121" t="n">
-        <v>720</v>
+        <v>504</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>0.645093</v>
+        <v>0.648145</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -8283,13 +8295,13 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C122" t="n">
-        <v>701</v>
+        <v>504</v>
       </c>
       <c r="D122" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>0.81238</v>
+        <v>0.658578</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -8353,13 +8365,19 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C123" t="n">
-        <v>4</v>
+        <v>504</v>
       </c>
       <c r="D123" t="n">
-        <v>88</v>
-      </c>
-      <c r="E123" t="inlineStr"/>
-      <c r="F123" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.65907</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Multi_index_HWMId</t>
+        </is>
+      </c>
       <c r="G123" t="inlineStr">
         <is>
           <t>ERA5</t>
@@ -8417,17 +8435,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C124" t="n">
-        <v>559</v>
+        <v>504</v>
       </c>
       <c r="D124" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>0.692956</v>
+        <v>0.648145</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Multi_index_HWMId_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -8487,17 +8505,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C125" t="n">
-        <v>558</v>
+        <v>504</v>
       </c>
       <c r="D125" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>0.727341</v>
+        <v>0.658578</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -8557,17 +8575,17 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C126" t="n">
-        <v>595</v>
+        <v>504</v>
       </c>
       <c r="D126" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>0.786332</v>
+        <v>0.65907</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Pseudo_HWMId_pop_NL</t>
+          <t>Multi_index_HWMId</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -8627,13 +8645,13 @@
         <v>0.174603174603175</v>
       </c>
       <c r="C127" t="n">
-        <v>704</v>
+        <v>504</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>0.661479</v>
+        <v>0.648145</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
@@ -8905,7 +8923,7 @@
         <v>19</v>
       </c>
       <c r="E131" t="n">
-        <v>0.803191</v>
+        <v>0.812176</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -9441,7 +9459,7 @@
         <v>5</v>
       </c>
       <c r="E139" t="n">
-        <v>0.710882</v>
+        <v>0.721186</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -10445,7 +10463,7 @@
         <v>5</v>
       </c>
       <c r="E154" t="n">
-        <v>0.692327</v>
+        <v>0.703962</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -10913,7 +10931,7 @@
         <v>34</v>
       </c>
       <c r="E161" t="n">
-        <v>0.798743</v>
+        <v>0.800221</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
@@ -11449,7 +11467,7 @@
         <v>5</v>
       </c>
       <c r="E169" t="n">
-        <v>0.721419</v>
+        <v>0.728106</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -11643,7 +11661,7 @@
         <v>16</v>
       </c>
       <c r="E172" t="n">
-        <v>0.7911589999999999</v>
+        <v>0.80022</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>

</xml_diff>